<commit_message>
feat: update cell order
</commit_message>
<xml_diff>
--- a/bulls.xlsx
+++ b/bulls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Registration Code</t>
   </si>
@@ -40,25 +40,16 @@
     <t xml:space="preserve">Freddie The Biggie</t>
   </si>
   <si>
-    <t xml:space="preserve">NE23ED</t>
-  </si>
-  <si>
     <t xml:space="preserve">002</t>
   </si>
   <si>
     <t xml:space="preserve">Arnold II</t>
   </si>
   <si>
-    <t xml:space="preserve">25.8</t>
-  </si>
-  <si>
     <t xml:space="preserve">001</t>
   </si>
   <si>
     <t xml:space="preserve">March</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.5</t>
   </si>
   <si>
     <t xml:space="preserve">000</t>
@@ -75,7 +66,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -99,19 +90,32 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,17 +152,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -170,6 +178,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF1F1F1F"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -180,17 +248,13 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.77"/>
-  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -204,7 +268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -212,49 +276,49 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>42129</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>42139</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="n">
+        <v>41743</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>41733</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="2" t="n">
+        <v>41346</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>41336</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="2" t="n">
-        <v>40941</v>
+        <v>40951</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>

</xml_diff>